<commit_message>
QueueManagement stack, testing deploy
</commit_message>
<xml_diff>
--- a/Resources.xlsx
+++ b/Resources.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Diego Naranjo\Desktop\1. Projects\serverless_etl\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B77EFDB7-FDF2-4CBB-B40B-EBF50EEF3CC2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A90E9F9-0686-4557-9067-C6518F38F958}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" activeTab="1" xr2:uid="{8CF66506-2549-4E97-BAA5-AA2C619381FD}"/>
   </bookViews>
@@ -656,26 +656,36 @@
     <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -686,25 +696,15 @@
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1573,7 +1573,7 @@
   <dimension ref="A1:G46"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8:D12"/>
+      <selection activeCell="D13" sqref="D8:D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1588,17 +1588,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A1" s="15" t="s">
+      <c r="A1" s="29" t="s">
         <v>85</v>
       </c>
-      <c r="B1" s="15"/>
-      <c r="C1" s="15"/>
-      <c r="D1" s="15"/>
-      <c r="E1" s="16" t="s">
+      <c r="B1" s="29"/>
+      <c r="C1" s="29"/>
+      <c r="D1" s="29"/>
+      <c r="E1" s="30" t="s">
         <v>86</v>
       </c>
-      <c r="F1" s="16"/>
-      <c r="G1" s="16"/>
+      <c r="F1" s="30"/>
+      <c r="G1" s="30"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
@@ -1624,15 +1624,15 @@
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A3" s="18" t="s">
+      <c r="A3" s="16" t="s">
         <v>142</v>
       </c>
-      <c r="B3" s="18" t="s">
+      <c r="B3" s="16" t="s">
         <v>105</v>
       </c>
-      <c r="C3" s="18"/>
-      <c r="D3" s="20"/>
-      <c r="E3" s="1" t="s">
+      <c r="C3" s="16"/>
+      <c r="D3" s="25"/>
+      <c r="E3" s="14" t="s">
         <v>10</v>
       </c>
       <c r="F3" t="s">
@@ -1640,23 +1640,23 @@
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A4" s="18"/>
-      <c r="B4" s="18"/>
-      <c r="C4" s="18"/>
-      <c r="D4" s="20"/>
-      <c r="E4" s="1" t="s">
+      <c r="A4" s="16"/>
+      <c r="B4" s="16"/>
+      <c r="C4" s="16"/>
+      <c r="D4" s="25"/>
+      <c r="E4" s="14" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A5" s="17" t="s">
+      <c r="A5" s="31" t="s">
         <v>89</v>
       </c>
-      <c r="B5" s="18" t="s">
+      <c r="B5" s="16" t="s">
         <v>93</v>
       </c>
-      <c r="C5" s="18"/>
-      <c r="D5" s="19" t="s">
+      <c r="C5" s="16"/>
+      <c r="D5" s="18" t="s">
         <v>136</v>
       </c>
       <c r="E5" s="14" t="s">
@@ -1667,34 +1667,34 @@
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A6" s="17"/>
-      <c r="B6" s="18"/>
-      <c r="C6" s="18"/>
-      <c r="D6" s="19"/>
+      <c r="A6" s="31"/>
+      <c r="B6" s="16"/>
+      <c r="C6" s="16"/>
+      <c r="D6" s="18"/>
       <c r="E6" s="14" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A7" s="17"/>
-      <c r="B7" s="18"/>
-      <c r="C7" s="18"/>
-      <c r="D7" s="19"/>
+      <c r="A7" s="31"/>
+      <c r="B7" s="16"/>
+      <c r="C7" s="16"/>
+      <c r="D7" s="18"/>
       <c r="E7" s="14" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A8" s="29" t="s">
+      <c r="A8" s="19" t="s">
         <v>90</v>
       </c>
-      <c r="B8" s="18" t="s">
+      <c r="B8" s="16" t="s">
         <v>93</v>
       </c>
-      <c r="C8" s="18" t="s">
+      <c r="C8" s="16" t="s">
         <v>93</v>
       </c>
-      <c r="D8" s="19" t="s">
+      <c r="D8" s="18" t="s">
         <v>140</v>
       </c>
       <c r="E8" s="1" t="s">
@@ -1708,10 +1708,10 @@
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A9" s="29"/>
-      <c r="B9" s="18"/>
-      <c r="C9" s="18"/>
-      <c r="D9" s="26"/>
+      <c r="A9" s="19"/>
+      <c r="B9" s="16"/>
+      <c r="C9" s="16"/>
+      <c r="D9" s="17"/>
       <c r="E9" s="1" t="s">
         <v>27</v>
       </c>
@@ -1723,19 +1723,19 @@
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A10" s="29"/>
-      <c r="B10" s="18"/>
-      <c r="C10" s="18"/>
-      <c r="D10" s="26"/>
+      <c r="A10" s="19"/>
+      <c r="B10" s="16"/>
+      <c r="C10" s="16"/>
+      <c r="D10" s="17"/>
       <c r="E10" s="1" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A11" s="29"/>
-      <c r="B11" s="18"/>
-      <c r="C11" s="18"/>
-      <c r="D11" s="26"/>
+      <c r="A11" s="19"/>
+      <c r="B11" s="16"/>
+      <c r="C11" s="16"/>
+      <c r="D11" s="17"/>
       <c r="E11" s="1" t="s">
         <v>30</v>
       </c>
@@ -1744,10 +1744,10 @@
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A12" s="29"/>
-      <c r="B12" s="18"/>
-      <c r="C12" s="18"/>
-      <c r="D12" s="26"/>
+      <c r="A12" s="19"/>
+      <c r="B12" s="16"/>
+      <c r="C12" s="16"/>
+      <c r="D12" s="17"/>
       <c r="E12" s="1" t="s">
         <v>62</v>
       </c>
@@ -1759,16 +1759,16 @@
       </c>
     </row>
     <row r="13" spans="1:7" ht="29" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="30" t="s">
+      <c r="A13" s="20" t="s">
         <v>94</v>
       </c>
-      <c r="B13" s="18" t="s">
+      <c r="B13" s="16" t="s">
         <v>90</v>
       </c>
-      <c r="C13" s="19" t="s">
+      <c r="C13" s="18" t="s">
         <v>139</v>
       </c>
-      <c r="D13" s="26" t="s">
+      <c r="D13" s="17" t="s">
         <v>96</v>
       </c>
       <c r="E13" s="1" t="s">
@@ -1779,10 +1779,10 @@
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A14" s="30"/>
-      <c r="B14" s="18"/>
-      <c r="C14" s="19"/>
-      <c r="D14" s="26"/>
+      <c r="A14" s="20"/>
+      <c r="B14" s="16"/>
+      <c r="C14" s="18"/>
+      <c r="D14" s="17"/>
       <c r="E14" s="1" t="s">
         <v>56</v>
       </c>
@@ -1791,10 +1791,10 @@
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A15" s="30"/>
-      <c r="B15" s="18"/>
-      <c r="C15" s="19"/>
-      <c r="D15" s="26"/>
+      <c r="A15" s="20"/>
+      <c r="B15" s="16"/>
+      <c r="C15" s="18"/>
+      <c r="D15" s="17"/>
       <c r="E15" s="1" t="s">
         <v>73</v>
       </c>
@@ -1803,10 +1803,10 @@
       </c>
     </row>
     <row r="16" spans="1:7" ht="29" x14ac:dyDescent="0.35">
-      <c r="A16" s="30"/>
-      <c r="B16" s="18"/>
-      <c r="C16" s="19"/>
-      <c r="D16" s="26"/>
+      <c r="A16" s="20"/>
+      <c r="B16" s="16"/>
+      <c r="C16" s="18"/>
+      <c r="D16" s="17"/>
       <c r="E16" s="1" t="s">
         <v>76</v>
       </c>
@@ -1818,10 +1818,10 @@
       </c>
     </row>
     <row r="17" spans="1:7" ht="29" x14ac:dyDescent="0.35">
-      <c r="A17" s="30"/>
-      <c r="B17" s="18"/>
-      <c r="C17" s="19"/>
-      <c r="D17" s="26"/>
+      <c r="A17" s="20"/>
+      <c r="B17" s="16"/>
+      <c r="C17" s="18"/>
+      <c r="D17" s="17"/>
       <c r="E17" s="1" t="s">
         <v>79</v>
       </c>
@@ -1833,10 +1833,10 @@
       </c>
     </row>
     <row r="18" spans="1:7" ht="29" x14ac:dyDescent="0.35">
-      <c r="A18" s="30"/>
-      <c r="B18" s="18"/>
-      <c r="C18" s="19"/>
-      <c r="D18" s="26"/>
+      <c r="A18" s="20"/>
+      <c r="B18" s="16"/>
+      <c r="C18" s="18"/>
+      <c r="D18" s="17"/>
       <c r="E18" s="1" t="s">
         <v>80</v>
       </c>
@@ -1848,10 +1848,10 @@
       </c>
     </row>
     <row r="19" spans="1:7" ht="29" x14ac:dyDescent="0.35">
-      <c r="A19" s="30"/>
-      <c r="B19" s="18"/>
-      <c r="C19" s="19"/>
-      <c r="D19" s="26"/>
+      <c r="A19" s="20"/>
+      <c r="B19" s="16"/>
+      <c r="C19" s="18"/>
+      <c r="D19" s="17"/>
       <c r="E19" s="1" t="s">
         <v>81</v>
       </c>
@@ -1863,10 +1863,10 @@
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A20" s="30"/>
-      <c r="B20" s="18"/>
-      <c r="C20" s="19"/>
-      <c r="D20" s="26"/>
+      <c r="A20" s="20"/>
+      <c r="B20" s="16"/>
+      <c r="C20" s="18"/>
+      <c r="D20" s="17"/>
       <c r="E20" s="1" t="s">
         <v>61</v>
       </c>
@@ -1875,10 +1875,10 @@
       </c>
     </row>
     <row r="21" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A21" s="30"/>
-      <c r="B21" s="18"/>
-      <c r="C21" s="19"/>
-      <c r="D21" s="26"/>
+      <c r="A21" s="20"/>
+      <c r="B21" s="16"/>
+      <c r="C21" s="18"/>
+      <c r="D21" s="17"/>
       <c r="E21" s="1" t="s">
         <v>58</v>
       </c>
@@ -1890,10 +1890,10 @@
       </c>
     </row>
     <row r="22" spans="1:7" ht="29" x14ac:dyDescent="0.35">
-      <c r="A22" s="30"/>
-      <c r="B22" s="18"/>
-      <c r="C22" s="19"/>
-      <c r="D22" s="26"/>
+      <c r="A22" s="20"/>
+      <c r="B22" s="16"/>
+      <c r="C22" s="18"/>
+      <c r="D22" s="17"/>
       <c r="E22" s="9" t="s">
         <v>71</v>
       </c>
@@ -1903,19 +1903,19 @@
       <c r="G22" s="1"/>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A23" s="21" t="s">
+      <c r="A23" s="24" t="s">
         <v>105</v>
       </c>
-      <c r="B23" s="18" t="s">
+      <c r="B23" s="16" t="s">
         <v>93</v>
       </c>
-      <c r="C23" s="20" t="s">
+      <c r="C23" s="25" t="s">
         <v>93</v>
       </c>
-      <c r="D23" s="22" t="s">
+      <c r="D23" s="26" t="s">
         <v>106</v>
       </c>
-      <c r="E23" s="31" t="s">
+      <c r="E23" s="15" t="s">
         <v>0</v>
       </c>
       <c r="F23" s="5" t="s">
@@ -1923,11 +1923,11 @@
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A24" s="21"/>
-      <c r="B24" s="18"/>
-      <c r="C24" s="20"/>
-      <c r="D24" s="23"/>
-      <c r="E24" s="31" t="s">
+      <c r="A24" s="24"/>
+      <c r="B24" s="16"/>
+      <c r="C24" s="25"/>
+      <c r="D24" s="27"/>
+      <c r="E24" s="15" t="s">
         <v>5</v>
       </c>
       <c r="F24" s="5" t="s">
@@ -1935,16 +1935,16 @@
       </c>
     </row>
     <row r="25" spans="1:7" ht="29" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A25" s="24" t="s">
+      <c r="A25" s="28" t="s">
         <v>113</v>
       </c>
-      <c r="B25" s="18" t="s">
+      <c r="B25" s="16" t="s">
         <v>93</v>
       </c>
-      <c r="C25" s="18" t="s">
+      <c r="C25" s="16" t="s">
         <v>93</v>
       </c>
-      <c r="D25" s="19" t="s">
+      <c r="D25" s="18" t="s">
         <v>114</v>
       </c>
       <c r="E25" s="1" t="s">
@@ -1958,10 +1958,10 @@
       </c>
     </row>
     <row r="26" spans="1:7" ht="29" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A26" s="24"/>
-      <c r="B26" s="18"/>
-      <c r="C26" s="18"/>
-      <c r="D26" s="19"/>
+      <c r="A26" s="28"/>
+      <c r="B26" s="16"/>
+      <c r="C26" s="16"/>
+      <c r="D26" s="18"/>
       <c r="E26" s="1" t="s">
         <v>48</v>
       </c>
@@ -1973,16 +1973,16 @@
       </c>
     </row>
     <row r="27" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A27" s="28" t="s">
+      <c r="A27" s="23" t="s">
         <v>111</v>
       </c>
-      <c r="B27" s="19" t="s">
+      <c r="B27" s="18" t="s">
         <v>112</v>
       </c>
-      <c r="C27" s="19" t="s">
+      <c r="C27" s="18" t="s">
         <v>115</v>
       </c>
-      <c r="D27" s="26" t="s">
+      <c r="D27" s="17" t="s">
         <v>109</v>
       </c>
       <c r="E27" t="s">
@@ -1993,10 +1993,10 @@
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A28" s="28"/>
-      <c r="B28" s="19"/>
-      <c r="C28" s="19"/>
-      <c r="D28" s="26"/>
+      <c r="A28" s="23"/>
+      <c r="B28" s="18"/>
+      <c r="C28" s="18"/>
+      <c r="D28" s="17"/>
       <c r="E28" t="s">
         <v>16</v>
       </c>
@@ -2005,10 +2005,10 @@
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A29" s="28"/>
-      <c r="B29" s="19"/>
-      <c r="C29" s="19"/>
-      <c r="D29" s="26"/>
+      <c r="A29" s="23"/>
+      <c r="B29" s="18"/>
+      <c r="C29" s="18"/>
+      <c r="D29" s="17"/>
       <c r="E29" t="s">
         <v>19</v>
       </c>
@@ -2017,10 +2017,10 @@
       </c>
     </row>
     <row r="30" spans="1:7" ht="58" x14ac:dyDescent="0.35">
-      <c r="A30" s="28"/>
-      <c r="B30" s="19"/>
-      <c r="C30" s="19"/>
-      <c r="D30" s="26"/>
+      <c r="A30" s="23"/>
+      <c r="B30" s="18"/>
+      <c r="C30" s="18"/>
+      <c r="D30" s="17"/>
       <c r="E30" s="1" t="s">
         <v>20</v>
       </c>
@@ -2029,10 +2029,10 @@
       </c>
     </row>
     <row r="31" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A31" s="28"/>
-      <c r="B31" s="19"/>
-      <c r="C31" s="19"/>
-      <c r="D31" s="26"/>
+      <c r="A31" s="23"/>
+      <c r="B31" s="18"/>
+      <c r="C31" s="18"/>
+      <c r="D31" s="17"/>
       <c r="E31" s="1" t="s">
         <v>21</v>
       </c>
@@ -2041,10 +2041,10 @@
       </c>
     </row>
     <row r="32" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A32" s="28"/>
-      <c r="B32" s="19"/>
-      <c r="C32" s="19"/>
-      <c r="D32" s="26"/>
+      <c r="A32" s="23"/>
+      <c r="B32" s="18"/>
+      <c r="C32" s="18"/>
+      <c r="D32" s="17"/>
       <c r="E32" s="1" t="s">
         <v>22</v>
       </c>
@@ -2053,10 +2053,10 @@
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A33" s="28"/>
-      <c r="B33" s="19"/>
-      <c r="C33" s="19"/>
-      <c r="D33" s="26"/>
+      <c r="A33" s="23"/>
+      <c r="B33" s="18"/>
+      <c r="C33" s="18"/>
+      <c r="D33" s="17"/>
       <c r="E33" t="s">
         <v>6</v>
       </c>
@@ -2065,10 +2065,10 @@
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A34" s="28"/>
-      <c r="B34" s="19"/>
-      <c r="C34" s="19"/>
-      <c r="D34" s="26"/>
+      <c r="A34" s="23"/>
+      <c r="B34" s="18"/>
+      <c r="C34" s="18"/>
+      <c r="D34" s="17"/>
       <c r="E34" t="s">
         <v>8</v>
       </c>
@@ -2077,16 +2077,16 @@
       </c>
     </row>
     <row r="35" spans="1:7" ht="29" x14ac:dyDescent="0.35">
-      <c r="A35" s="27" t="s">
+      <c r="A35" s="22" t="s">
         <v>118</v>
       </c>
-      <c r="B35" s="19" t="s">
+      <c r="B35" s="18" t="s">
         <v>119</v>
       </c>
-      <c r="C35" s="19" t="s">
+      <c r="C35" s="18" t="s">
         <v>120</v>
       </c>
-      <c r="D35" s="18" t="s">
+      <c r="D35" s="16" t="s">
         <v>93</v>
       </c>
       <c r="E35" s="1" t="s">
@@ -2100,10 +2100,10 @@
       </c>
     </row>
     <row r="36" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A36" s="27"/>
-      <c r="B36" s="19"/>
-      <c r="C36" s="26"/>
-      <c r="D36" s="18"/>
+      <c r="A36" s="22"/>
+      <c r="B36" s="18"/>
+      <c r="C36" s="17"/>
+      <c r="D36" s="16"/>
       <c r="E36" s="9" t="s">
         <v>39</v>
       </c>
@@ -2112,10 +2112,10 @@
       </c>
     </row>
     <row r="37" spans="1:7" ht="29" x14ac:dyDescent="0.35">
-      <c r="A37" s="27"/>
-      <c r="B37" s="19"/>
-      <c r="C37" s="26"/>
-      <c r="D37" s="18"/>
+      <c r="A37" s="22"/>
+      <c r="B37" s="18"/>
+      <c r="C37" s="17"/>
+      <c r="D37" s="16"/>
       <c r="E37" s="9" t="s">
         <v>41</v>
       </c>
@@ -2124,10 +2124,10 @@
       </c>
     </row>
     <row r="38" spans="1:7" ht="29" x14ac:dyDescent="0.35">
-      <c r="A38" s="27"/>
-      <c r="B38" s="19"/>
-      <c r="C38" s="26"/>
-      <c r="D38" s="18"/>
+      <c r="A38" s="22"/>
+      <c r="B38" s="18"/>
+      <c r="C38" s="17"/>
+      <c r="D38" s="16"/>
       <c r="E38" s="9" t="s">
         <v>43</v>
       </c>
@@ -2136,10 +2136,10 @@
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A39" s="27"/>
-      <c r="B39" s="19"/>
-      <c r="C39" s="26"/>
-      <c r="D39" s="18"/>
+      <c r="A39" s="22"/>
+      <c r="B39" s="18"/>
+      <c r="C39" s="17"/>
+      <c r="D39" s="16"/>
       <c r="E39" t="s">
         <v>44</v>
       </c>
@@ -2148,10 +2148,10 @@
       </c>
     </row>
     <row r="40" spans="1:7" ht="29" x14ac:dyDescent="0.35">
-      <c r="A40" s="27"/>
-      <c r="B40" s="19"/>
-      <c r="C40" s="26"/>
-      <c r="D40" s="18"/>
+      <c r="A40" s="22"/>
+      <c r="B40" s="18"/>
+      <c r="C40" s="17"/>
+      <c r="D40" s="16"/>
       <c r="E40" t="s">
         <v>45</v>
       </c>
@@ -2160,16 +2160,16 @@
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A41" s="25" t="s">
+      <c r="A41" s="21" t="s">
         <v>126</v>
       </c>
-      <c r="B41" s="19" t="s">
+      <c r="B41" s="18" t="s">
         <v>127</v>
       </c>
-      <c r="C41" s="19" t="s">
+      <c r="C41" s="18" t="s">
         <v>129</v>
       </c>
-      <c r="D41" s="26" t="s">
+      <c r="D41" s="17" t="s">
         <v>141</v>
       </c>
       <c r="E41" t="s">
@@ -2183,10 +2183,10 @@
       </c>
     </row>
     <row r="42" spans="1:7" ht="29" x14ac:dyDescent="0.35">
-      <c r="A42" s="25"/>
-      <c r="B42" s="26"/>
-      <c r="C42" s="26"/>
-      <c r="D42" s="26"/>
+      <c r="A42" s="21"/>
+      <c r="B42" s="17"/>
+      <c r="C42" s="17"/>
+      <c r="D42" s="17"/>
       <c r="E42" s="1" t="s">
         <v>18</v>
       </c>
@@ -2195,16 +2195,16 @@
       </c>
     </row>
     <row r="43" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A43" s="18" t="s">
+      <c r="A43" s="16" t="s">
         <v>130</v>
       </c>
-      <c r="B43" s="19" t="s">
+      <c r="B43" s="18" t="s">
         <v>131</v>
       </c>
-      <c r="C43" s="19" t="s">
+      <c r="C43" s="18" t="s">
         <v>134</v>
       </c>
-      <c r="D43" s="18" t="s">
+      <c r="D43" s="16" t="s">
         <v>93</v>
       </c>
       <c r="E43" s="9" t="s">
@@ -2218,10 +2218,10 @@
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A44" s="18"/>
-      <c r="B44" s="26"/>
-      <c r="C44" s="26"/>
-      <c r="D44" s="18"/>
+      <c r="A44" s="16"/>
+      <c r="B44" s="17"/>
+      <c r="C44" s="17"/>
+      <c r="D44" s="16"/>
       <c r="E44" t="s">
         <v>36</v>
       </c>
@@ -2230,16 +2230,16 @@
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A45" s="18" t="s">
+      <c r="A45" s="16" t="s">
         <v>135</v>
       </c>
-      <c r="B45" s="18" t="s">
+      <c r="B45" s="16" t="s">
         <v>89</v>
       </c>
-      <c r="C45" s="26" t="s">
+      <c r="C45" s="17" t="s">
         <v>136</v>
       </c>
-      <c r="D45" s="18" t="s">
+      <c r="D45" s="16" t="s">
         <v>93</v>
       </c>
       <c r="E45" t="s">
@@ -2247,10 +2247,10 @@
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A46" s="18"/>
-      <c r="B46" s="18"/>
-      <c r="C46" s="26"/>
-      <c r="D46" s="18"/>
+      <c r="A46" s="16"/>
+      <c r="B46" s="16"/>
+      <c r="C46" s="17"/>
+      <c r="D46" s="16"/>
       <c r="E46" t="s">
         <v>69</v>
       </c>
@@ -2263,20 +2263,22 @@
     </row>
   </sheetData>
   <mergeCells count="46">
-    <mergeCell ref="A45:A46"/>
-    <mergeCell ref="B45:B46"/>
-    <mergeCell ref="C45:C46"/>
-    <mergeCell ref="D45:D46"/>
-    <mergeCell ref="A43:A44"/>
-    <mergeCell ref="B43:B44"/>
-    <mergeCell ref="C43:C44"/>
-    <mergeCell ref="D43:D44"/>
-    <mergeCell ref="A8:A12"/>
-    <mergeCell ref="B8:B12"/>
-    <mergeCell ref="C8:C12"/>
-    <mergeCell ref="D8:D12"/>
-    <mergeCell ref="A13:A22"/>
-    <mergeCell ref="B13:B22"/>
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="E1:G1"/>
+    <mergeCell ref="A5:A7"/>
+    <mergeCell ref="A3:A4"/>
+    <mergeCell ref="B5:B7"/>
+    <mergeCell ref="C3:C4"/>
+    <mergeCell ref="C5:C7"/>
+    <mergeCell ref="D5:D7"/>
+    <mergeCell ref="D3:D4"/>
+    <mergeCell ref="B3:B4"/>
+    <mergeCell ref="A23:A24"/>
+    <mergeCell ref="B23:B24"/>
+    <mergeCell ref="C23:C24"/>
+    <mergeCell ref="D23:D24"/>
+    <mergeCell ref="B25:B26"/>
+    <mergeCell ref="A25:A26"/>
     <mergeCell ref="A41:A42"/>
     <mergeCell ref="B41:B42"/>
     <mergeCell ref="C41:C42"/>
@@ -2293,22 +2295,20 @@
     <mergeCell ref="B27:B34"/>
     <mergeCell ref="C27:C34"/>
     <mergeCell ref="D27:D34"/>
-    <mergeCell ref="A23:A24"/>
-    <mergeCell ref="B23:B24"/>
-    <mergeCell ref="C23:C24"/>
-    <mergeCell ref="D23:D24"/>
-    <mergeCell ref="B25:B26"/>
-    <mergeCell ref="A25:A26"/>
-    <mergeCell ref="A1:D1"/>
-    <mergeCell ref="E1:G1"/>
-    <mergeCell ref="A5:A7"/>
-    <mergeCell ref="A3:A4"/>
-    <mergeCell ref="B5:B7"/>
-    <mergeCell ref="C3:C4"/>
-    <mergeCell ref="C5:C7"/>
-    <mergeCell ref="D5:D7"/>
-    <mergeCell ref="D3:D4"/>
-    <mergeCell ref="B3:B4"/>
+    <mergeCell ref="A8:A12"/>
+    <mergeCell ref="B8:B12"/>
+    <mergeCell ref="C8:C12"/>
+    <mergeCell ref="D8:D12"/>
+    <mergeCell ref="A13:A22"/>
+    <mergeCell ref="B13:B22"/>
+    <mergeCell ref="A45:A46"/>
+    <mergeCell ref="B45:B46"/>
+    <mergeCell ref="C45:C46"/>
+    <mergeCell ref="D45:D46"/>
+    <mergeCell ref="A43:A44"/>
+    <mergeCell ref="B43:B44"/>
+    <mergeCell ref="C43:C44"/>
+    <mergeCell ref="D43:D44"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
MonitoringNObservability template and QueueManagement outputs
</commit_message>
<xml_diff>
--- a/Resources.xlsx
+++ b/Resources.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Diego Naranjo\Desktop\1. Projects\serverless_etl\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A90E9F9-0686-4557-9067-C6518F38F958}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32DDE6CE-BB4D-4659-AB8D-6E08484E9AC5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" activeTab="1" xr2:uid="{8CF66506-2549-4E97-BAA5-AA2C619381FD}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="291" uniqueCount="143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="290" uniqueCount="143">
   <si>
     <t>LambdaLayerParameter</t>
   </si>
@@ -657,35 +657,26 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -696,13 +687,22 @@
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1572,8 +1572,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7DB30289-44B1-413E-86BC-E0029586D835}">
   <dimension ref="A1:G46"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D8:D22"/>
+    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13:E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1588,17 +1588,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A1" s="29" t="s">
+      <c r="A1" s="16" t="s">
         <v>85</v>
       </c>
-      <c r="B1" s="29"/>
-      <c r="C1" s="29"/>
-      <c r="D1" s="29"/>
-      <c r="E1" s="30" t="s">
+      <c r="B1" s="16"/>
+      <c r="C1" s="16"/>
+      <c r="D1" s="16"/>
+      <c r="E1" s="17" t="s">
         <v>86</v>
       </c>
-      <c r="F1" s="30"/>
-      <c r="G1" s="30"/>
+      <c r="F1" s="17"/>
+      <c r="G1" s="17"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
@@ -1624,14 +1624,14 @@
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A3" s="16" t="s">
+      <c r="A3" s="19" t="s">
         <v>142</v>
       </c>
-      <c r="B3" s="16" t="s">
+      <c r="B3" s="19" t="s">
         <v>105</v>
       </c>
-      <c r="C3" s="16"/>
-      <c r="D3" s="25"/>
+      <c r="C3" s="19"/>
+      <c r="D3" s="21"/>
       <c r="E3" s="14" t="s">
         <v>10</v>
       </c>
@@ -1640,23 +1640,23 @@
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A4" s="16"/>
-      <c r="B4" s="16"/>
-      <c r="C4" s="16"/>
-      <c r="D4" s="25"/>
+      <c r="A4" s="19"/>
+      <c r="B4" s="19"/>
+      <c r="C4" s="19"/>
+      <c r="D4" s="21"/>
       <c r="E4" s="14" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A5" s="31" t="s">
+      <c r="A5" s="18" t="s">
         <v>89</v>
       </c>
-      <c r="B5" s="16" t="s">
+      <c r="B5" s="19" t="s">
         <v>93</v>
       </c>
-      <c r="C5" s="16"/>
-      <c r="D5" s="18" t="s">
+      <c r="C5" s="19"/>
+      <c r="D5" s="20" t="s">
         <v>136</v>
       </c>
       <c r="E5" s="14" t="s">
@@ -1667,37 +1667,37 @@
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A6" s="31"/>
-      <c r="B6" s="16"/>
-      <c r="C6" s="16"/>
-      <c r="D6" s="18"/>
+      <c r="A6" s="18"/>
+      <c r="B6" s="19"/>
+      <c r="C6" s="19"/>
+      <c r="D6" s="20"/>
       <c r="E6" s="14" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A7" s="31"/>
-      <c r="B7" s="16"/>
-      <c r="C7" s="16"/>
-      <c r="D7" s="18"/>
+      <c r="A7" s="18"/>
+      <c r="B7" s="19"/>
+      <c r="C7" s="19"/>
+      <c r="D7" s="20"/>
       <c r="E7" s="14" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A8" s="19" t="s">
+      <c r="A8" s="30" t="s">
         <v>90</v>
       </c>
-      <c r="B8" s="16" t="s">
+      <c r="B8" s="19" t="s">
         <v>93</v>
       </c>
-      <c r="C8" s="16" t="s">
+      <c r="C8" s="19" t="s">
         <v>93</v>
       </c>
-      <c r="D8" s="18" t="s">
+      <c r="D8" s="20" t="s">
         <v>140</v>
       </c>
-      <c r="E8" s="1" t="s">
+      <c r="E8" s="14" t="s">
         <v>51</v>
       </c>
       <c r="F8" t="s">
@@ -1708,11 +1708,11 @@
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A9" s="19"/>
-      <c r="B9" s="16"/>
-      <c r="C9" s="16"/>
-      <c r="D9" s="17"/>
-      <c r="E9" s="1" t="s">
+      <c r="A9" s="30"/>
+      <c r="B9" s="19"/>
+      <c r="C9" s="19"/>
+      <c r="D9" s="27"/>
+      <c r="E9" s="14" t="s">
         <v>27</v>
       </c>
       <c r="F9" t="s">
@@ -1723,20 +1723,20 @@
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A10" s="19"/>
-      <c r="B10" s="16"/>
-      <c r="C10" s="16"/>
-      <c r="D10" s="17"/>
-      <c r="E10" s="1" t="s">
+      <c r="A10" s="30"/>
+      <c r="B10" s="19"/>
+      <c r="C10" s="19"/>
+      <c r="D10" s="27"/>
+      <c r="E10" s="14" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A11" s="19"/>
-      <c r="B11" s="16"/>
-      <c r="C11" s="16"/>
-      <c r="D11" s="17"/>
-      <c r="E11" s="1" t="s">
+      <c r="A11" s="30"/>
+      <c r="B11" s="19"/>
+      <c r="C11" s="19"/>
+      <c r="D11" s="27"/>
+      <c r="E11" s="14" t="s">
         <v>30</v>
       </c>
       <c r="F11" t="s">
@@ -1744,11 +1744,11 @@
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A12" s="19"/>
-      <c r="B12" s="16"/>
-      <c r="C12" s="16"/>
-      <c r="D12" s="17"/>
-      <c r="E12" s="1" t="s">
+      <c r="A12" s="30"/>
+      <c r="B12" s="19"/>
+      <c r="C12" s="19"/>
+      <c r="D12" s="27"/>
+      <c r="E12" s="14" t="s">
         <v>62</v>
       </c>
       <c r="F12" t="s">
@@ -1759,19 +1759,17 @@
       </c>
     </row>
     <row r="13" spans="1:7" ht="29" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="20" t="s">
+      <c r="A13" s="31" t="s">
         <v>94</v>
       </c>
-      <c r="B13" s="16" t="s">
+      <c r="B13" s="19" t="s">
         <v>90</v>
       </c>
-      <c r="C13" s="18" t="s">
+      <c r="C13" s="20" t="s">
         <v>139</v>
       </c>
-      <c r="D13" s="17" t="s">
-        <v>96</v>
-      </c>
-      <c r="E13" s="1" t="s">
+      <c r="D13" s="27"/>
+      <c r="E13" s="14" t="s">
         <v>54</v>
       </c>
       <c r="F13" s="5" t="s">
@@ -1779,11 +1777,11 @@
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A14" s="20"/>
-      <c r="B14" s="16"/>
-      <c r="C14" s="18"/>
-      <c r="D14" s="17"/>
-      <c r="E14" s="1" t="s">
+      <c r="A14" s="31"/>
+      <c r="B14" s="19"/>
+      <c r="C14" s="20"/>
+      <c r="D14" s="27"/>
+      <c r="E14" s="14" t="s">
         <v>56</v>
       </c>
       <c r="F14" t="s">
@@ -1791,11 +1789,11 @@
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A15" s="20"/>
-      <c r="B15" s="16"/>
-      <c r="C15" s="18"/>
-      <c r="D15" s="17"/>
-      <c r="E15" s="1" t="s">
+      <c r="A15" s="31"/>
+      <c r="B15" s="19"/>
+      <c r="C15" s="20"/>
+      <c r="D15" s="27"/>
+      <c r="E15" s="14" t="s">
         <v>73</v>
       </c>
       <c r="F15" t="s">
@@ -1803,11 +1801,11 @@
       </c>
     </row>
     <row r="16" spans="1:7" ht="29" x14ac:dyDescent="0.35">
-      <c r="A16" s="20"/>
-      <c r="B16" s="16"/>
-      <c r="C16" s="18"/>
-      <c r="D16" s="17"/>
-      <c r="E16" s="1" t="s">
+      <c r="A16" s="31"/>
+      <c r="B16" s="19"/>
+      <c r="C16" s="20"/>
+      <c r="D16" s="27"/>
+      <c r="E16" s="14" t="s">
         <v>76</v>
       </c>
       <c r="F16" s="5" t="s">
@@ -1818,11 +1816,11 @@
       </c>
     </row>
     <row r="17" spans="1:7" ht="29" x14ac:dyDescent="0.35">
-      <c r="A17" s="20"/>
-      <c r="B17" s="16"/>
-      <c r="C17" s="18"/>
-      <c r="D17" s="17"/>
-      <c r="E17" s="1" t="s">
+      <c r="A17" s="31"/>
+      <c r="B17" s="19"/>
+      <c r="C17" s="20"/>
+      <c r="D17" s="27"/>
+      <c r="E17" s="14" t="s">
         <v>79</v>
       </c>
       <c r="F17" s="5" t="s">
@@ -1833,11 +1831,11 @@
       </c>
     </row>
     <row r="18" spans="1:7" ht="29" x14ac:dyDescent="0.35">
-      <c r="A18" s="20"/>
-      <c r="B18" s="16"/>
-      <c r="C18" s="18"/>
-      <c r="D18" s="17"/>
-      <c r="E18" s="1" t="s">
+      <c r="A18" s="31"/>
+      <c r="B18" s="19"/>
+      <c r="C18" s="20"/>
+      <c r="D18" s="27"/>
+      <c r="E18" s="14" t="s">
         <v>80</v>
       </c>
       <c r="F18" s="5" t="s">
@@ -1848,11 +1846,11 @@
       </c>
     </row>
     <row r="19" spans="1:7" ht="29" x14ac:dyDescent="0.35">
-      <c r="A19" s="20"/>
-      <c r="B19" s="16"/>
-      <c r="C19" s="18"/>
-      <c r="D19" s="17"/>
-      <c r="E19" s="1" t="s">
+      <c r="A19" s="31"/>
+      <c r="B19" s="19"/>
+      <c r="C19" s="20"/>
+      <c r="D19" s="27"/>
+      <c r="E19" s="14" t="s">
         <v>81</v>
       </c>
       <c r="F19" s="5" t="s">
@@ -1863,11 +1861,11 @@
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A20" s="20"/>
-      <c r="B20" s="16"/>
-      <c r="C20" s="18"/>
-      <c r="D20" s="17"/>
-      <c r="E20" s="1" t="s">
+      <c r="A20" s="31"/>
+      <c r="B20" s="19"/>
+      <c r="C20" s="20"/>
+      <c r="D20" s="27"/>
+      <c r="E20" s="14" t="s">
         <v>61</v>
       </c>
       <c r="F20" s="5" t="s">
@@ -1875,11 +1873,11 @@
       </c>
     </row>
     <row r="21" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A21" s="20"/>
-      <c r="B21" s="16"/>
-      <c r="C21" s="18"/>
-      <c r="D21" s="17"/>
-      <c r="E21" s="1" t="s">
+      <c r="A21" s="31"/>
+      <c r="B21" s="19"/>
+      <c r="C21" s="20"/>
+      <c r="D21" s="27"/>
+      <c r="E21" s="14" t="s">
         <v>58</v>
       </c>
       <c r="F21" s="5" t="s">
@@ -1890,11 +1888,11 @@
       </c>
     </row>
     <row r="22" spans="1:7" ht="29" x14ac:dyDescent="0.35">
-      <c r="A22" s="20"/>
-      <c r="B22" s="16"/>
-      <c r="C22" s="18"/>
-      <c r="D22" s="17"/>
-      <c r="E22" s="9" t="s">
+      <c r="A22" s="31"/>
+      <c r="B22" s="19"/>
+      <c r="C22" s="20"/>
+      <c r="D22" s="27"/>
+      <c r="E22" s="14" t="s">
         <v>71</v>
       </c>
       <c r="F22" s="5" t="s">
@@ -1903,16 +1901,16 @@
       <c r="G22" s="1"/>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A23" s="24" t="s">
+      <c r="A23" s="22" t="s">
         <v>105</v>
       </c>
-      <c r="B23" s="16" t="s">
+      <c r="B23" s="19" t="s">
         <v>93</v>
       </c>
-      <c r="C23" s="25" t="s">
+      <c r="C23" s="21" t="s">
         <v>93</v>
       </c>
-      <c r="D23" s="26" t="s">
+      <c r="D23" s="23" t="s">
         <v>106</v>
       </c>
       <c r="E23" s="15" t="s">
@@ -1923,10 +1921,10 @@
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A24" s="24"/>
-      <c r="B24" s="16"/>
-      <c r="C24" s="25"/>
-      <c r="D24" s="27"/>
+      <c r="A24" s="22"/>
+      <c r="B24" s="19"/>
+      <c r="C24" s="21"/>
+      <c r="D24" s="24"/>
       <c r="E24" s="15" t="s">
         <v>5</v>
       </c>
@@ -1935,16 +1933,16 @@
       </c>
     </row>
     <row r="25" spans="1:7" ht="29" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A25" s="28" t="s">
+      <c r="A25" s="25" t="s">
         <v>113</v>
       </c>
-      <c r="B25" s="16" t="s">
+      <c r="B25" s="19" t="s">
         <v>93</v>
       </c>
-      <c r="C25" s="16" t="s">
+      <c r="C25" s="19" t="s">
         <v>93</v>
       </c>
-      <c r="D25" s="18" t="s">
+      <c r="D25" s="20" t="s">
         <v>114</v>
       </c>
       <c r="E25" s="1" t="s">
@@ -1958,10 +1956,10 @@
       </c>
     </row>
     <row r="26" spans="1:7" ht="29" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A26" s="28"/>
-      <c r="B26" s="16"/>
-      <c r="C26" s="16"/>
-      <c r="D26" s="18"/>
+      <c r="A26" s="25"/>
+      <c r="B26" s="19"/>
+      <c r="C26" s="19"/>
+      <c r="D26" s="20"/>
       <c r="E26" s="1" t="s">
         <v>48</v>
       </c>
@@ -1973,16 +1971,16 @@
       </c>
     </row>
     <row r="27" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A27" s="23" t="s">
+      <c r="A27" s="29" t="s">
         <v>111</v>
       </c>
-      <c r="B27" s="18" t="s">
+      <c r="B27" s="20" t="s">
         <v>112</v>
       </c>
-      <c r="C27" s="18" t="s">
+      <c r="C27" s="20" t="s">
         <v>115</v>
       </c>
-      <c r="D27" s="17" t="s">
+      <c r="D27" s="27" t="s">
         <v>109</v>
       </c>
       <c r="E27" t="s">
@@ -1993,10 +1991,10 @@
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A28" s="23"/>
-      <c r="B28" s="18"/>
-      <c r="C28" s="18"/>
-      <c r="D28" s="17"/>
+      <c r="A28" s="29"/>
+      <c r="B28" s="20"/>
+      <c r="C28" s="20"/>
+      <c r="D28" s="27"/>
       <c r="E28" t="s">
         <v>16</v>
       </c>
@@ -2005,10 +2003,10 @@
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A29" s="23"/>
-      <c r="B29" s="18"/>
-      <c r="C29" s="18"/>
-      <c r="D29" s="17"/>
+      <c r="A29" s="29"/>
+      <c r="B29" s="20"/>
+      <c r="C29" s="20"/>
+      <c r="D29" s="27"/>
       <c r="E29" t="s">
         <v>19</v>
       </c>
@@ -2017,10 +2015,10 @@
       </c>
     </row>
     <row r="30" spans="1:7" ht="58" x14ac:dyDescent="0.35">
-      <c r="A30" s="23"/>
-      <c r="B30" s="18"/>
-      <c r="C30" s="18"/>
-      <c r="D30" s="17"/>
+      <c r="A30" s="29"/>
+      <c r="B30" s="20"/>
+      <c r="C30" s="20"/>
+      <c r="D30" s="27"/>
       <c r="E30" s="1" t="s">
         <v>20</v>
       </c>
@@ -2029,10 +2027,10 @@
       </c>
     </row>
     <row r="31" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A31" s="23"/>
-      <c r="B31" s="18"/>
-      <c r="C31" s="18"/>
-      <c r="D31" s="17"/>
+      <c r="A31" s="29"/>
+      <c r="B31" s="20"/>
+      <c r="C31" s="20"/>
+      <c r="D31" s="27"/>
       <c r="E31" s="1" t="s">
         <v>21</v>
       </c>
@@ -2041,10 +2039,10 @@
       </c>
     </row>
     <row r="32" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A32" s="23"/>
-      <c r="B32" s="18"/>
-      <c r="C32" s="18"/>
-      <c r="D32" s="17"/>
+      <c r="A32" s="29"/>
+      <c r="B32" s="20"/>
+      <c r="C32" s="20"/>
+      <c r="D32" s="27"/>
       <c r="E32" s="1" t="s">
         <v>22</v>
       </c>
@@ -2053,10 +2051,10 @@
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A33" s="23"/>
-      <c r="B33" s="18"/>
-      <c r="C33" s="18"/>
-      <c r="D33" s="17"/>
+      <c r="A33" s="29"/>
+      <c r="B33" s="20"/>
+      <c r="C33" s="20"/>
+      <c r="D33" s="27"/>
       <c r="E33" t="s">
         <v>6</v>
       </c>
@@ -2065,10 +2063,10 @@
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A34" s="23"/>
-      <c r="B34" s="18"/>
-      <c r="C34" s="18"/>
-      <c r="D34" s="17"/>
+      <c r="A34" s="29"/>
+      <c r="B34" s="20"/>
+      <c r="C34" s="20"/>
+      <c r="D34" s="27"/>
       <c r="E34" t="s">
         <v>8</v>
       </c>
@@ -2077,16 +2075,16 @@
       </c>
     </row>
     <row r="35" spans="1:7" ht="29" x14ac:dyDescent="0.35">
-      <c r="A35" s="22" t="s">
+      <c r="A35" s="28" t="s">
         <v>118</v>
       </c>
-      <c r="B35" s="18" t="s">
+      <c r="B35" s="20" t="s">
         <v>119</v>
       </c>
-      <c r="C35" s="18" t="s">
+      <c r="C35" s="20" t="s">
         <v>120</v>
       </c>
-      <c r="D35" s="16" t="s">
+      <c r="D35" s="19" t="s">
         <v>93</v>
       </c>
       <c r="E35" s="1" t="s">
@@ -2100,10 +2098,10 @@
       </c>
     </row>
     <row r="36" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A36" s="22"/>
-      <c r="B36" s="18"/>
-      <c r="C36" s="17"/>
-      <c r="D36" s="16"/>
+      <c r="A36" s="28"/>
+      <c r="B36" s="20"/>
+      <c r="C36" s="27"/>
+      <c r="D36" s="19"/>
       <c r="E36" s="9" t="s">
         <v>39</v>
       </c>
@@ -2112,10 +2110,10 @@
       </c>
     </row>
     <row r="37" spans="1:7" ht="29" x14ac:dyDescent="0.35">
-      <c r="A37" s="22"/>
-      <c r="B37" s="18"/>
-      <c r="C37" s="17"/>
-      <c r="D37" s="16"/>
+      <c r="A37" s="28"/>
+      <c r="B37" s="20"/>
+      <c r="C37" s="27"/>
+      <c r="D37" s="19"/>
       <c r="E37" s="9" t="s">
         <v>41</v>
       </c>
@@ -2124,10 +2122,10 @@
       </c>
     </row>
     <row r="38" spans="1:7" ht="29" x14ac:dyDescent="0.35">
-      <c r="A38" s="22"/>
-      <c r="B38" s="18"/>
-      <c r="C38" s="17"/>
-      <c r="D38" s="16"/>
+      <c r="A38" s="28"/>
+      <c r="B38" s="20"/>
+      <c r="C38" s="27"/>
+      <c r="D38" s="19"/>
       <c r="E38" s="9" t="s">
         <v>43</v>
       </c>
@@ -2136,10 +2134,10 @@
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A39" s="22"/>
-      <c r="B39" s="18"/>
-      <c r="C39" s="17"/>
-      <c r="D39" s="16"/>
+      <c r="A39" s="28"/>
+      <c r="B39" s="20"/>
+      <c r="C39" s="27"/>
+      <c r="D39" s="19"/>
       <c r="E39" t="s">
         <v>44</v>
       </c>
@@ -2148,10 +2146,10 @@
       </c>
     </row>
     <row r="40" spans="1:7" ht="29" x14ac:dyDescent="0.35">
-      <c r="A40" s="22"/>
-      <c r="B40" s="18"/>
-      <c r="C40" s="17"/>
-      <c r="D40" s="16"/>
+      <c r="A40" s="28"/>
+      <c r="B40" s="20"/>
+      <c r="C40" s="27"/>
+      <c r="D40" s="19"/>
       <c r="E40" t="s">
         <v>45</v>
       </c>
@@ -2160,16 +2158,16 @@
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A41" s="21" t="s">
+      <c r="A41" s="26" t="s">
         <v>126</v>
       </c>
-      <c r="B41" s="18" t="s">
+      <c r="B41" s="20" t="s">
         <v>127</v>
       </c>
-      <c r="C41" s="18" t="s">
+      <c r="C41" s="20" t="s">
         <v>129</v>
       </c>
-      <c r="D41" s="17" t="s">
+      <c r="D41" s="27" t="s">
         <v>141</v>
       </c>
       <c r="E41" t="s">
@@ -2183,10 +2181,10 @@
       </c>
     </row>
     <row r="42" spans="1:7" ht="29" x14ac:dyDescent="0.35">
-      <c r="A42" s="21"/>
-      <c r="B42" s="17"/>
-      <c r="C42" s="17"/>
-      <c r="D42" s="17"/>
+      <c r="A42" s="26"/>
+      <c r="B42" s="27"/>
+      <c r="C42" s="27"/>
+      <c r="D42" s="27"/>
       <c r="E42" s="1" t="s">
         <v>18</v>
       </c>
@@ -2195,16 +2193,16 @@
       </c>
     </row>
     <row r="43" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A43" s="16" t="s">
+      <c r="A43" s="19" t="s">
         <v>130</v>
       </c>
-      <c r="B43" s="18" t="s">
+      <c r="B43" s="20" t="s">
         <v>131</v>
       </c>
-      <c r="C43" s="18" t="s">
+      <c r="C43" s="20" t="s">
         <v>134</v>
       </c>
-      <c r="D43" s="16" t="s">
+      <c r="D43" s="19" t="s">
         <v>93</v>
       </c>
       <c r="E43" s="9" t="s">
@@ -2218,10 +2216,10 @@
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A44" s="16"/>
-      <c r="B44" s="17"/>
-      <c r="C44" s="17"/>
-      <c r="D44" s="16"/>
+      <c r="A44" s="19"/>
+      <c r="B44" s="27"/>
+      <c r="C44" s="27"/>
+      <c r="D44" s="19"/>
       <c r="E44" t="s">
         <v>36</v>
       </c>
@@ -2230,16 +2228,16 @@
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A45" s="16" t="s">
+      <c r="A45" s="19" t="s">
         <v>135</v>
       </c>
-      <c r="B45" s="16" t="s">
+      <c r="B45" s="19" t="s">
         <v>89</v>
       </c>
-      <c r="C45" s="17" t="s">
+      <c r="C45" s="27" t="s">
         <v>136</v>
       </c>
-      <c r="D45" s="16" t="s">
+      <c r="D45" s="19" t="s">
         <v>93</v>
       </c>
       <c r="E45" t="s">
@@ -2247,10 +2245,10 @@
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A46" s="16"/>
-      <c r="B46" s="16"/>
-      <c r="C46" s="17"/>
-      <c r="D46" s="16"/>
+      <c r="A46" s="19"/>
+      <c r="B46" s="19"/>
+      <c r="C46" s="27"/>
+      <c r="D46" s="19"/>
       <c r="E46" t="s">
         <v>69</v>
       </c>
@@ -2263,22 +2261,20 @@
     </row>
   </sheetData>
   <mergeCells count="46">
-    <mergeCell ref="A1:D1"/>
-    <mergeCell ref="E1:G1"/>
-    <mergeCell ref="A5:A7"/>
-    <mergeCell ref="A3:A4"/>
-    <mergeCell ref="B5:B7"/>
-    <mergeCell ref="C3:C4"/>
-    <mergeCell ref="C5:C7"/>
-    <mergeCell ref="D5:D7"/>
-    <mergeCell ref="D3:D4"/>
-    <mergeCell ref="B3:B4"/>
-    <mergeCell ref="A23:A24"/>
-    <mergeCell ref="B23:B24"/>
-    <mergeCell ref="C23:C24"/>
-    <mergeCell ref="D23:D24"/>
-    <mergeCell ref="B25:B26"/>
-    <mergeCell ref="A25:A26"/>
+    <mergeCell ref="A45:A46"/>
+    <mergeCell ref="B45:B46"/>
+    <mergeCell ref="C45:C46"/>
+    <mergeCell ref="D45:D46"/>
+    <mergeCell ref="A43:A44"/>
+    <mergeCell ref="B43:B44"/>
+    <mergeCell ref="C43:C44"/>
+    <mergeCell ref="D43:D44"/>
+    <mergeCell ref="A8:A12"/>
+    <mergeCell ref="B8:B12"/>
+    <mergeCell ref="C8:C12"/>
+    <mergeCell ref="D8:D12"/>
+    <mergeCell ref="A13:A22"/>
+    <mergeCell ref="B13:B22"/>
     <mergeCell ref="A41:A42"/>
     <mergeCell ref="B41:B42"/>
     <mergeCell ref="C41:C42"/>
@@ -2295,20 +2291,22 @@
     <mergeCell ref="B27:B34"/>
     <mergeCell ref="C27:C34"/>
     <mergeCell ref="D27:D34"/>
-    <mergeCell ref="A8:A12"/>
-    <mergeCell ref="B8:B12"/>
-    <mergeCell ref="C8:C12"/>
-    <mergeCell ref="D8:D12"/>
-    <mergeCell ref="A13:A22"/>
-    <mergeCell ref="B13:B22"/>
-    <mergeCell ref="A45:A46"/>
-    <mergeCell ref="B45:B46"/>
-    <mergeCell ref="C45:C46"/>
-    <mergeCell ref="D45:D46"/>
-    <mergeCell ref="A43:A44"/>
-    <mergeCell ref="B43:B44"/>
-    <mergeCell ref="C43:C44"/>
-    <mergeCell ref="D43:D44"/>
+    <mergeCell ref="A23:A24"/>
+    <mergeCell ref="B23:B24"/>
+    <mergeCell ref="C23:C24"/>
+    <mergeCell ref="D23:D24"/>
+    <mergeCell ref="B25:B26"/>
+    <mergeCell ref="A25:A26"/>
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="E1:G1"/>
+    <mergeCell ref="A5:A7"/>
+    <mergeCell ref="A3:A4"/>
+    <mergeCell ref="B5:B7"/>
+    <mergeCell ref="C3:C4"/>
+    <mergeCell ref="C5:C7"/>
+    <mergeCell ref="D5:D7"/>
+    <mergeCell ref="D3:D4"/>
+    <mergeCell ref="B3:B4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
layers required to store custom ETL libraries and code
</commit_message>
<xml_diff>
--- a/Resources.xlsx
+++ b/Resources.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Diego Naranjo\Desktop\1. Projects\serverless_etl\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32DDE6CE-BB4D-4659-AB8D-6E08484E9AC5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE22A6CB-DFBE-46E4-83A0-16F8E722DBF6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" activeTab="1" xr2:uid="{8CF66506-2549-4E97-BAA5-AA2C619381FD}"/>
   </bookViews>
@@ -657,26 +657,35 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -687,22 +696,13 @@
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1572,8 +1572,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7DB30289-44B1-413E-86BC-E0029586D835}">
   <dimension ref="A1:G46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13:E22"/>
+    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="E30" sqref="E30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1588,17 +1588,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="29" t="s">
         <v>85</v>
       </c>
-      <c r="B1" s="16"/>
-      <c r="C1" s="16"/>
-      <c r="D1" s="16"/>
-      <c r="E1" s="17" t="s">
+      <c r="B1" s="29"/>
+      <c r="C1" s="29"/>
+      <c r="D1" s="29"/>
+      <c r="E1" s="30" t="s">
         <v>86</v>
       </c>
-      <c r="F1" s="17"/>
-      <c r="G1" s="17"/>
+      <c r="F1" s="30"/>
+      <c r="G1" s="30"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
@@ -1624,14 +1624,14 @@
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A3" s="19" t="s">
+      <c r="A3" s="16" t="s">
         <v>142</v>
       </c>
-      <c r="B3" s="19" t="s">
+      <c r="B3" s="16" t="s">
         <v>105</v>
       </c>
-      <c r="C3" s="19"/>
-      <c r="D3" s="21"/>
+      <c r="C3" s="16"/>
+      <c r="D3" s="25"/>
       <c r="E3" s="14" t="s">
         <v>10</v>
       </c>
@@ -1640,23 +1640,23 @@
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A4" s="19"/>
-      <c r="B4" s="19"/>
-      <c r="C4" s="19"/>
-      <c r="D4" s="21"/>
+      <c r="A4" s="16"/>
+      <c r="B4" s="16"/>
+      <c r="C4" s="16"/>
+      <c r="D4" s="25"/>
       <c r="E4" s="14" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A5" s="18" t="s">
+      <c r="A5" s="31" t="s">
         <v>89</v>
       </c>
-      <c r="B5" s="19" t="s">
+      <c r="B5" s="16" t="s">
         <v>93</v>
       </c>
-      <c r="C5" s="19"/>
-      <c r="D5" s="20" t="s">
+      <c r="C5" s="16"/>
+      <c r="D5" s="18" t="s">
         <v>136</v>
       </c>
       <c r="E5" s="14" t="s">
@@ -1667,34 +1667,34 @@
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A6" s="18"/>
-      <c r="B6" s="19"/>
-      <c r="C6" s="19"/>
-      <c r="D6" s="20"/>
+      <c r="A6" s="31"/>
+      <c r="B6" s="16"/>
+      <c r="C6" s="16"/>
+      <c r="D6" s="18"/>
       <c r="E6" s="14" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A7" s="18"/>
-      <c r="B7" s="19"/>
-      <c r="C7" s="19"/>
-      <c r="D7" s="20"/>
+      <c r="A7" s="31"/>
+      <c r="B7" s="16"/>
+      <c r="C7" s="16"/>
+      <c r="D7" s="18"/>
       <c r="E7" s="14" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A8" s="30" t="s">
+      <c r="A8" s="19" t="s">
         <v>90</v>
       </c>
-      <c r="B8" s="19" t="s">
+      <c r="B8" s="16" t="s">
         <v>93</v>
       </c>
-      <c r="C8" s="19" t="s">
+      <c r="C8" s="16" t="s">
         <v>93</v>
       </c>
-      <c r="D8" s="20" t="s">
+      <c r="D8" s="18" t="s">
         <v>140</v>
       </c>
       <c r="E8" s="14" t="s">
@@ -1708,10 +1708,10 @@
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A9" s="30"/>
-      <c r="B9" s="19"/>
-      <c r="C9" s="19"/>
-      <c r="D9" s="27"/>
+      <c r="A9" s="19"/>
+      <c r="B9" s="16"/>
+      <c r="C9" s="16"/>
+      <c r="D9" s="17"/>
       <c r="E9" s="14" t="s">
         <v>27</v>
       </c>
@@ -1723,19 +1723,19 @@
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A10" s="30"/>
-      <c r="B10" s="19"/>
-      <c r="C10" s="19"/>
-      <c r="D10" s="27"/>
+      <c r="A10" s="19"/>
+      <c r="B10" s="16"/>
+      <c r="C10" s="16"/>
+      <c r="D10" s="17"/>
       <c r="E10" s="14" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A11" s="30"/>
-      <c r="B11" s="19"/>
-      <c r="C11" s="19"/>
-      <c r="D11" s="27"/>
+      <c r="A11" s="19"/>
+      <c r="B11" s="16"/>
+      <c r="C11" s="16"/>
+      <c r="D11" s="17"/>
       <c r="E11" s="14" t="s">
         <v>30</v>
       </c>
@@ -1744,10 +1744,10 @@
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A12" s="30"/>
-      <c r="B12" s="19"/>
-      <c r="C12" s="19"/>
-      <c r="D12" s="27"/>
+      <c r="A12" s="19"/>
+      <c r="B12" s="16"/>
+      <c r="C12" s="16"/>
+      <c r="D12" s="17"/>
       <c r="E12" s="14" t="s">
         <v>62</v>
       </c>
@@ -1759,16 +1759,16 @@
       </c>
     </row>
     <row r="13" spans="1:7" ht="29" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="31" t="s">
+      <c r="A13" s="20" t="s">
         <v>94</v>
       </c>
-      <c r="B13" s="19" t="s">
+      <c r="B13" s="16" t="s">
         <v>90</v>
       </c>
-      <c r="C13" s="20" t="s">
+      <c r="C13" s="18" t="s">
         <v>139</v>
       </c>
-      <c r="D13" s="27"/>
+      <c r="D13" s="17"/>
       <c r="E13" s="14" t="s">
         <v>54</v>
       </c>
@@ -1777,10 +1777,10 @@
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A14" s="31"/>
-      <c r="B14" s="19"/>
-      <c r="C14" s="20"/>
-      <c r="D14" s="27"/>
+      <c r="A14" s="20"/>
+      <c r="B14" s="16"/>
+      <c r="C14" s="18"/>
+      <c r="D14" s="17"/>
       <c r="E14" s="14" t="s">
         <v>56</v>
       </c>
@@ -1789,10 +1789,10 @@
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A15" s="31"/>
-      <c r="B15" s="19"/>
-      <c r="C15" s="20"/>
-      <c r="D15" s="27"/>
+      <c r="A15" s="20"/>
+      <c r="B15" s="16"/>
+      <c r="C15" s="18"/>
+      <c r="D15" s="17"/>
       <c r="E15" s="14" t="s">
         <v>73</v>
       </c>
@@ -1801,10 +1801,10 @@
       </c>
     </row>
     <row r="16" spans="1:7" ht="29" x14ac:dyDescent="0.35">
-      <c r="A16" s="31"/>
-      <c r="B16" s="19"/>
-      <c r="C16" s="20"/>
-      <c r="D16" s="27"/>
+      <c r="A16" s="20"/>
+      <c r="B16" s="16"/>
+      <c r="C16" s="18"/>
+      <c r="D16" s="17"/>
       <c r="E16" s="14" t="s">
         <v>76</v>
       </c>
@@ -1816,10 +1816,10 @@
       </c>
     </row>
     <row r="17" spans="1:7" ht="29" x14ac:dyDescent="0.35">
-      <c r="A17" s="31"/>
-      <c r="B17" s="19"/>
-      <c r="C17" s="20"/>
-      <c r="D17" s="27"/>
+      <c r="A17" s="20"/>
+      <c r="B17" s="16"/>
+      <c r="C17" s="18"/>
+      <c r="D17" s="17"/>
       <c r="E17" s="14" t="s">
         <v>79</v>
       </c>
@@ -1831,10 +1831,10 @@
       </c>
     </row>
     <row r="18" spans="1:7" ht="29" x14ac:dyDescent="0.35">
-      <c r="A18" s="31"/>
-      <c r="B18" s="19"/>
-      <c r="C18" s="20"/>
-      <c r="D18" s="27"/>
+      <c r="A18" s="20"/>
+      <c r="B18" s="16"/>
+      <c r="C18" s="18"/>
+      <c r="D18" s="17"/>
       <c r="E18" s="14" t="s">
         <v>80</v>
       </c>
@@ -1846,10 +1846,10 @@
       </c>
     </row>
     <row r="19" spans="1:7" ht="29" x14ac:dyDescent="0.35">
-      <c r="A19" s="31"/>
-      <c r="B19" s="19"/>
-      <c r="C19" s="20"/>
-      <c r="D19" s="27"/>
+      <c r="A19" s="20"/>
+      <c r="B19" s="16"/>
+      <c r="C19" s="18"/>
+      <c r="D19" s="17"/>
       <c r="E19" s="14" t="s">
         <v>81</v>
       </c>
@@ -1861,10 +1861,10 @@
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A20" s="31"/>
-      <c r="B20" s="19"/>
-      <c r="C20" s="20"/>
-      <c r="D20" s="27"/>
+      <c r="A20" s="20"/>
+      <c r="B20" s="16"/>
+      <c r="C20" s="18"/>
+      <c r="D20" s="17"/>
       <c r="E20" s="14" t="s">
         <v>61</v>
       </c>
@@ -1873,10 +1873,10 @@
       </c>
     </row>
     <row r="21" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A21" s="31"/>
-      <c r="B21" s="19"/>
-      <c r="C21" s="20"/>
-      <c r="D21" s="27"/>
+      <c r="A21" s="20"/>
+      <c r="B21" s="16"/>
+      <c r="C21" s="18"/>
+      <c r="D21" s="17"/>
       <c r="E21" s="14" t="s">
         <v>58</v>
       </c>
@@ -1888,10 +1888,10 @@
       </c>
     </row>
     <row r="22" spans="1:7" ht="29" x14ac:dyDescent="0.35">
-      <c r="A22" s="31"/>
-      <c r="B22" s="19"/>
-      <c r="C22" s="20"/>
-      <c r="D22" s="27"/>
+      <c r="A22" s="20"/>
+      <c r="B22" s="16"/>
+      <c r="C22" s="18"/>
+      <c r="D22" s="17"/>
       <c r="E22" s="14" t="s">
         <v>71</v>
       </c>
@@ -1901,16 +1901,16 @@
       <c r="G22" s="1"/>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A23" s="22" t="s">
+      <c r="A23" s="24" t="s">
         <v>105</v>
       </c>
-      <c r="B23" s="19" t="s">
+      <c r="B23" s="16" t="s">
         <v>93</v>
       </c>
-      <c r="C23" s="21" t="s">
+      <c r="C23" s="25" t="s">
         <v>93</v>
       </c>
-      <c r="D23" s="23" t="s">
+      <c r="D23" s="26" t="s">
         <v>106</v>
       </c>
       <c r="E23" s="15" t="s">
@@ -1921,10 +1921,10 @@
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A24" s="22"/>
-      <c r="B24" s="19"/>
-      <c r="C24" s="21"/>
-      <c r="D24" s="24"/>
+      <c r="A24" s="24"/>
+      <c r="B24" s="16"/>
+      <c r="C24" s="25"/>
+      <c r="D24" s="27"/>
       <c r="E24" s="15" t="s">
         <v>5</v>
       </c>
@@ -1933,19 +1933,19 @@
       </c>
     </row>
     <row r="25" spans="1:7" ht="29" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A25" s="25" t="s">
+      <c r="A25" s="28" t="s">
         <v>113</v>
       </c>
-      <c r="B25" s="19" t="s">
+      <c r="B25" s="16" t="s">
         <v>93</v>
       </c>
-      <c r="C25" s="19" t="s">
+      <c r="C25" s="16" t="s">
         <v>93</v>
       </c>
-      <c r="D25" s="20" t="s">
+      <c r="D25" s="18" t="s">
         <v>114</v>
       </c>
-      <c r="E25" s="1" t="s">
+      <c r="E25" s="15" t="s">
         <v>32</v>
       </c>
       <c r="F25" s="5" t="s">
@@ -1956,11 +1956,11 @@
       </c>
     </row>
     <row r="26" spans="1:7" ht="29" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A26" s="25"/>
-      <c r="B26" s="19"/>
-      <c r="C26" s="19"/>
-      <c r="D26" s="20"/>
-      <c r="E26" s="1" t="s">
+      <c r="A26" s="28"/>
+      <c r="B26" s="16"/>
+      <c r="C26" s="16"/>
+      <c r="D26" s="18"/>
+      <c r="E26" s="15" t="s">
         <v>48</v>
       </c>
       <c r="F26" s="5" t="s">
@@ -1971,16 +1971,16 @@
       </c>
     </row>
     <row r="27" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A27" s="29" t="s">
+      <c r="A27" s="23" t="s">
         <v>111</v>
       </c>
-      <c r="B27" s="20" t="s">
+      <c r="B27" s="18" t="s">
         <v>112</v>
       </c>
-      <c r="C27" s="20" t="s">
+      <c r="C27" s="18" t="s">
         <v>115</v>
       </c>
-      <c r="D27" s="27" t="s">
+      <c r="D27" s="17" t="s">
         <v>109</v>
       </c>
       <c r="E27" t="s">
@@ -1991,10 +1991,10 @@
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A28" s="29"/>
-      <c r="B28" s="20"/>
-      <c r="C28" s="20"/>
-      <c r="D28" s="27"/>
+      <c r="A28" s="23"/>
+      <c r="B28" s="18"/>
+      <c r="C28" s="18"/>
+      <c r="D28" s="17"/>
       <c r="E28" t="s">
         <v>16</v>
       </c>
@@ -2003,10 +2003,10 @@
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A29" s="29"/>
-      <c r="B29" s="20"/>
-      <c r="C29" s="20"/>
-      <c r="D29" s="27"/>
+      <c r="A29" s="23"/>
+      <c r="B29" s="18"/>
+      <c r="C29" s="18"/>
+      <c r="D29" s="17"/>
       <c r="E29" t="s">
         <v>19</v>
       </c>
@@ -2015,10 +2015,10 @@
       </c>
     </row>
     <row r="30" spans="1:7" ht="58" x14ac:dyDescent="0.35">
-      <c r="A30" s="29"/>
-      <c r="B30" s="20"/>
-      <c r="C30" s="20"/>
-      <c r="D30" s="27"/>
+      <c r="A30" s="23"/>
+      <c r="B30" s="18"/>
+      <c r="C30" s="18"/>
+      <c r="D30" s="17"/>
       <c r="E30" s="1" t="s">
         <v>20</v>
       </c>
@@ -2027,10 +2027,10 @@
       </c>
     </row>
     <row r="31" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A31" s="29"/>
-      <c r="B31" s="20"/>
-      <c r="C31" s="20"/>
-      <c r="D31" s="27"/>
+      <c r="A31" s="23"/>
+      <c r="B31" s="18"/>
+      <c r="C31" s="18"/>
+      <c r="D31" s="17"/>
       <c r="E31" s="1" t="s">
         <v>21</v>
       </c>
@@ -2039,10 +2039,10 @@
       </c>
     </row>
     <row r="32" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A32" s="29"/>
-      <c r="B32" s="20"/>
-      <c r="C32" s="20"/>
-      <c r="D32" s="27"/>
+      <c r="A32" s="23"/>
+      <c r="B32" s="18"/>
+      <c r="C32" s="18"/>
+      <c r="D32" s="17"/>
       <c r="E32" s="1" t="s">
         <v>22</v>
       </c>
@@ -2051,10 +2051,10 @@
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A33" s="29"/>
-      <c r="B33" s="20"/>
-      <c r="C33" s="20"/>
-      <c r="D33" s="27"/>
+      <c r="A33" s="23"/>
+      <c r="B33" s="18"/>
+      <c r="C33" s="18"/>
+      <c r="D33" s="17"/>
       <c r="E33" t="s">
         <v>6</v>
       </c>
@@ -2063,10 +2063,10 @@
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A34" s="29"/>
-      <c r="B34" s="20"/>
-      <c r="C34" s="20"/>
-      <c r="D34" s="27"/>
+      <c r="A34" s="23"/>
+      <c r="B34" s="18"/>
+      <c r="C34" s="18"/>
+      <c r="D34" s="17"/>
       <c r="E34" t="s">
         <v>8</v>
       </c>
@@ -2075,16 +2075,16 @@
       </c>
     </row>
     <row r="35" spans="1:7" ht="29" x14ac:dyDescent="0.35">
-      <c r="A35" s="28" t="s">
+      <c r="A35" s="22" t="s">
         <v>118</v>
       </c>
-      <c r="B35" s="20" t="s">
+      <c r="B35" s="18" t="s">
         <v>119</v>
       </c>
-      <c r="C35" s="20" t="s">
+      <c r="C35" s="18" t="s">
         <v>120</v>
       </c>
-      <c r="D35" s="19" t="s">
+      <c r="D35" s="16" t="s">
         <v>93</v>
       </c>
       <c r="E35" s="1" t="s">
@@ -2098,10 +2098,10 @@
       </c>
     </row>
     <row r="36" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A36" s="28"/>
-      <c r="B36" s="20"/>
-      <c r="C36" s="27"/>
-      <c r="D36" s="19"/>
+      <c r="A36" s="22"/>
+      <c r="B36" s="18"/>
+      <c r="C36" s="17"/>
+      <c r="D36" s="16"/>
       <c r="E36" s="9" t="s">
         <v>39</v>
       </c>
@@ -2110,10 +2110,10 @@
       </c>
     </row>
     <row r="37" spans="1:7" ht="29" x14ac:dyDescent="0.35">
-      <c r="A37" s="28"/>
-      <c r="B37" s="20"/>
-      <c r="C37" s="27"/>
-      <c r="D37" s="19"/>
+      <c r="A37" s="22"/>
+      <c r="B37" s="18"/>
+      <c r="C37" s="17"/>
+      <c r="D37" s="16"/>
       <c r="E37" s="9" t="s">
         <v>41</v>
       </c>
@@ -2122,10 +2122,10 @@
       </c>
     </row>
     <row r="38" spans="1:7" ht="29" x14ac:dyDescent="0.35">
-      <c r="A38" s="28"/>
-      <c r="B38" s="20"/>
-      <c r="C38" s="27"/>
-      <c r="D38" s="19"/>
+      <c r="A38" s="22"/>
+      <c r="B38" s="18"/>
+      <c r="C38" s="17"/>
+      <c r="D38" s="16"/>
       <c r="E38" s="9" t="s">
         <v>43</v>
       </c>
@@ -2134,10 +2134,10 @@
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A39" s="28"/>
-      <c r="B39" s="20"/>
-      <c r="C39" s="27"/>
-      <c r="D39" s="19"/>
+      <c r="A39" s="22"/>
+      <c r="B39" s="18"/>
+      <c r="C39" s="17"/>
+      <c r="D39" s="16"/>
       <c r="E39" t="s">
         <v>44</v>
       </c>
@@ -2146,10 +2146,10 @@
       </c>
     </row>
     <row r="40" spans="1:7" ht="29" x14ac:dyDescent="0.35">
-      <c r="A40" s="28"/>
-      <c r="B40" s="20"/>
-      <c r="C40" s="27"/>
-      <c r="D40" s="19"/>
+      <c r="A40" s="22"/>
+      <c r="B40" s="18"/>
+      <c r="C40" s="17"/>
+      <c r="D40" s="16"/>
       <c r="E40" t="s">
         <v>45</v>
       </c>
@@ -2158,16 +2158,16 @@
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A41" s="26" t="s">
+      <c r="A41" s="21" t="s">
         <v>126</v>
       </c>
-      <c r="B41" s="20" t="s">
+      <c r="B41" s="18" t="s">
         <v>127</v>
       </c>
-      <c r="C41" s="20" t="s">
+      <c r="C41" s="18" t="s">
         <v>129</v>
       </c>
-      <c r="D41" s="27" t="s">
+      <c r="D41" s="17" t="s">
         <v>141</v>
       </c>
       <c r="E41" t="s">
@@ -2181,10 +2181,10 @@
       </c>
     </row>
     <row r="42" spans="1:7" ht="29" x14ac:dyDescent="0.35">
-      <c r="A42" s="26"/>
-      <c r="B42" s="27"/>
-      <c r="C42" s="27"/>
-      <c r="D42" s="27"/>
+      <c r="A42" s="21"/>
+      <c r="B42" s="17"/>
+      <c r="C42" s="17"/>
+      <c r="D42" s="17"/>
       <c r="E42" s="1" t="s">
         <v>18</v>
       </c>
@@ -2193,16 +2193,16 @@
       </c>
     </row>
     <row r="43" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A43" s="19" t="s">
+      <c r="A43" s="16" t="s">
         <v>130</v>
       </c>
-      <c r="B43" s="20" t="s">
+      <c r="B43" s="18" t="s">
         <v>131</v>
       </c>
-      <c r="C43" s="20" t="s">
+      <c r="C43" s="18" t="s">
         <v>134</v>
       </c>
-      <c r="D43" s="19" t="s">
+      <c r="D43" s="16" t="s">
         <v>93</v>
       </c>
       <c r="E43" s="9" t="s">
@@ -2216,10 +2216,10 @@
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A44" s="19"/>
-      <c r="B44" s="27"/>
-      <c r="C44" s="27"/>
-      <c r="D44" s="19"/>
+      <c r="A44" s="16"/>
+      <c r="B44" s="17"/>
+      <c r="C44" s="17"/>
+      <c r="D44" s="16"/>
       <c r="E44" t="s">
         <v>36</v>
       </c>
@@ -2228,16 +2228,16 @@
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A45" s="19" t="s">
+      <c r="A45" s="16" t="s">
         <v>135</v>
       </c>
-      <c r="B45" s="19" t="s">
+      <c r="B45" s="16" t="s">
         <v>89</v>
       </c>
-      <c r="C45" s="27" t="s">
+      <c r="C45" s="17" t="s">
         <v>136</v>
       </c>
-      <c r="D45" s="19" t="s">
+      <c r="D45" s="16" t="s">
         <v>93</v>
       </c>
       <c r="E45" t="s">
@@ -2245,10 +2245,10 @@
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A46" s="19"/>
-      <c r="B46" s="19"/>
-      <c r="C46" s="27"/>
-      <c r="D46" s="19"/>
+      <c r="A46" s="16"/>
+      <c r="B46" s="16"/>
+      <c r="C46" s="17"/>
+      <c r="D46" s="16"/>
       <c r="E46" t="s">
         <v>69</v>
       </c>
@@ -2261,20 +2261,22 @@
     </row>
   </sheetData>
   <mergeCells count="46">
-    <mergeCell ref="A45:A46"/>
-    <mergeCell ref="B45:B46"/>
-    <mergeCell ref="C45:C46"/>
-    <mergeCell ref="D45:D46"/>
-    <mergeCell ref="A43:A44"/>
-    <mergeCell ref="B43:B44"/>
-    <mergeCell ref="C43:C44"/>
-    <mergeCell ref="D43:D44"/>
-    <mergeCell ref="A8:A12"/>
-    <mergeCell ref="B8:B12"/>
-    <mergeCell ref="C8:C12"/>
-    <mergeCell ref="D8:D12"/>
-    <mergeCell ref="A13:A22"/>
-    <mergeCell ref="B13:B22"/>
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="E1:G1"/>
+    <mergeCell ref="A5:A7"/>
+    <mergeCell ref="A3:A4"/>
+    <mergeCell ref="B5:B7"/>
+    <mergeCell ref="C3:C4"/>
+    <mergeCell ref="C5:C7"/>
+    <mergeCell ref="D5:D7"/>
+    <mergeCell ref="D3:D4"/>
+    <mergeCell ref="B3:B4"/>
+    <mergeCell ref="A23:A24"/>
+    <mergeCell ref="B23:B24"/>
+    <mergeCell ref="C23:C24"/>
+    <mergeCell ref="D23:D24"/>
+    <mergeCell ref="B25:B26"/>
+    <mergeCell ref="A25:A26"/>
     <mergeCell ref="A41:A42"/>
     <mergeCell ref="B41:B42"/>
     <mergeCell ref="C41:C42"/>
@@ -2291,22 +2293,20 @@
     <mergeCell ref="B27:B34"/>
     <mergeCell ref="C27:C34"/>
     <mergeCell ref="D27:D34"/>
-    <mergeCell ref="A23:A24"/>
-    <mergeCell ref="B23:B24"/>
-    <mergeCell ref="C23:C24"/>
-    <mergeCell ref="D23:D24"/>
-    <mergeCell ref="B25:B26"/>
-    <mergeCell ref="A25:A26"/>
-    <mergeCell ref="A1:D1"/>
-    <mergeCell ref="E1:G1"/>
-    <mergeCell ref="A5:A7"/>
-    <mergeCell ref="A3:A4"/>
-    <mergeCell ref="B5:B7"/>
-    <mergeCell ref="C3:C4"/>
-    <mergeCell ref="C5:C7"/>
-    <mergeCell ref="D5:D7"/>
-    <mergeCell ref="D3:D4"/>
-    <mergeCell ref="B3:B4"/>
+    <mergeCell ref="A8:A12"/>
+    <mergeCell ref="B8:B12"/>
+    <mergeCell ref="C8:C12"/>
+    <mergeCell ref="D8:D12"/>
+    <mergeCell ref="A13:A22"/>
+    <mergeCell ref="B13:B22"/>
+    <mergeCell ref="A45:A46"/>
+    <mergeCell ref="B45:B46"/>
+    <mergeCell ref="C45:C46"/>
+    <mergeCell ref="D45:D46"/>
+    <mergeCell ref="A43:A44"/>
+    <mergeCell ref="B43:B44"/>
+    <mergeCell ref="C43:C44"/>
+    <mergeCell ref="D43:D44"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>